<commit_message>
max_min test data added
</commit_message>
<xml_diff>
--- a/logs/gravity.xlsx
+++ b/logs/gravity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythonProjects\deepLearning\myCodes\gravity_optimizer\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F0454-FACC-49F0-9E5A-D6BE892F71FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5997CCDC-9C4D-49A0-8468-0CF59FD9186C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{32C8AF95-1429-4A21-8CF7-B38E1399F39E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>epochs</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>max_step_grad = z_score</t>
+  </si>
+  <si>
+    <t>max_step_grad = 1/(max_grad-min_grad+self.epsilon)</t>
   </si>
 </sst>
 </file>
@@ -14264,6 +14267,649 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>max_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$A$3:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$N$3:$N$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2.3027694225311199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2586250305175701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9639205932617101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.69606614112854</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4662382602691599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.22249507904052</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.03525698184967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86408096551895097</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73870247602462702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.62412256002426103</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.53597235679626398</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43687659502029402</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.35687324404716397</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.296150982379913</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.241215795278549</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.20251764357089899</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.159939751029014</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.13020826876163399</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.113895647227764</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8499804735183702E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.3440661430358803E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.3875906169414506E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.7438258081674499E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.1439322531223297E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.4517900794744401E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.2967006564140299E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2790429890155702E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.6234069615602403E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8777642175555201E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2647304236888802E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.5497399270534502E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6842882856726601E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.3679494857787999E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.6706651076674399E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.2398622706532399E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8463643267750698E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.45105952396988E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.9130390137433999E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.22592309489846E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.6287580132484401E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2325801886618099E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.3690935447812001E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2208929285407E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0713316500186899E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.2847088277339901E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.36198019608855E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.8996391966938903E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.16662429645657E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.9769149199128099E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.7704093419015399E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.48136084899306E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7.8989565372467006E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8.6336946114897693E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.1168524622917101E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>9.8036741837859102E-3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8.66168364882469E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.0448790900409204E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.3184653669595701E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.3734287396073298E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1314079165458599E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.1706529445946199E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.7819828875362804E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.6465428052469999E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.7559421509504301E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.5061445087194399E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.09932459890842E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.3701562099158703E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.7748803198337503E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.3161205723881704E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.2651176229119301E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.2543926499783902E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.1170655749738199E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.5495112687349302E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.2901436835527403E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.2806065864860998E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.3930583633482404E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.9995980486273696E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.0557285752147401E-3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.5057077873498201E-3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.9772616475820498E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7.8713977709412505E-3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.0218998957425302E-4</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.39324998599477E-4</c:v>
+                </c:pt>
+                <c:pt idx="83" formatCode="0.00E+00">
+                  <c:v>2.3290514945983799E-5</c:v>
+                </c:pt>
+                <c:pt idx="84" formatCode="0.00E+00">
+                  <c:v>1.4991532225394599E-5</c:v>
+                </c:pt>
+                <c:pt idx="85" formatCode="0.00E+00">
+                  <c:v>1.22376850413274E-5</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="0.00E+00">
+                  <c:v>1.04406317404937E-5</c:v>
+                </c:pt>
+                <c:pt idx="87" formatCode="0.00E+00">
+                  <c:v>9.1319379862397892E-6</c:v>
+                </c:pt>
+                <c:pt idx="88" formatCode="0.00E+00">
+                  <c:v>8.1310226960340498E-6</c:v>
+                </c:pt>
+                <c:pt idx="89" formatCode="0.00E+00">
+                  <c:v>7.3339556365681304E-6</c:v>
+                </c:pt>
+                <c:pt idx="90" formatCode="0.00E+00">
+                  <c:v>6.6808324845624097E-6</c:v>
+                </c:pt>
+                <c:pt idx="91" formatCode="0.00E+00">
+                  <c:v>6.1339046624197997E-6</c:v>
+                </c:pt>
+                <c:pt idx="92" formatCode="0.00E+00">
+                  <c:v>5.6691937970754199E-6</c:v>
+                </c:pt>
+                <c:pt idx="93" formatCode="0.00E+00">
+                  <c:v>5.2707268878293596E-6</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="0.00E+00">
+                  <c:v>4.9238369683734996E-6</c:v>
+                </c:pt>
+                <c:pt idx="95" formatCode="0.00E+00">
+                  <c:v>4.6196814764698502E-6</c:v>
+                </c:pt>
+                <c:pt idx="96" formatCode="0.00E+00">
+                  <c:v>4.3496561374922698E-6</c:v>
+                </c:pt>
+                <c:pt idx="97" formatCode="0.00E+00">
+                  <c:v>4.1098924157267902E-6</c:v>
+                </c:pt>
+                <c:pt idx="98" formatCode="0.00E+00">
+                  <c:v>3.8948614928813101E-6</c:v>
+                </c:pt>
+                <c:pt idx="99" formatCode="0.00E+00">
+                  <c:v>3.7005947888246699E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ED53-4F42-A0BD-1C7D1B071518}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -16602,6 +17248,649 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D876-4069-A2AA-C9B44965F3BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>max_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$A$3:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$P$3:$P$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2.3022925853729199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0786178112029998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8122906684875399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5514733791351301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.39426958560943</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1325269937515201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0254898071289</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.89834278821945102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83198076486587502</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.79875659942626898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72993385791778498</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76859366893768299</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.722639560699462</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.73433947563171298</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.86505204439163197</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.77807712554931596</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.87954413890838601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85024952888488703</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.91134178638458196</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96869343519210804</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.96055614948272705</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.98949795961380005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0180149078369101</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.98585760593414296</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0578082799911499</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99726057052612305</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1213850975036599</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1584111452102599</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1236149072646999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.08906114101409</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.17526471614837</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.03588771820068</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.16630411148071</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2954134941101001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.2055369615554801</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1399447917938199</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1890002489089899</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.1808214187621999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.2814165353775</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.1881618499755799</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2059458494186399</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.25268542766571</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2093030214309599</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.2619669437408401</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.24342000484466</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.2116824388503999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.32473564147949</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.3087188005447301</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.29738068580627</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.38581454753875</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.18995833396911</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.31305539608001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.27703416347503</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.2660480737686099</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.3768168687820399</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.2122414112091</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.3161154985427801</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.2984709739685001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.32701575756073</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.23300921916961</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.40980112552642</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3081873655319201</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.4868196249008101</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.3691926002502399</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.64860951900482</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.2998180389404199</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.52765369415283</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.2738339900970399</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.36833119392395</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.3437414169311499</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.41374015808105</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.4031784534454299</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.35831654071807</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.3287324905395499</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.46714067459106</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.4421035051345801</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.3833097219467101</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.4210299253463701</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.44810795783996</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.4834080934524501</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.26602470874786</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.39194107055664</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.4401205778121899</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.4550211429595901</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.46996474266052</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.4829174280166599</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.49461674690246</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.5052117109298699</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.5148837566375699</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.52382004261016</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.5321733951568599</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.5400135517120299</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.5473601818084699</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.5543675422668399</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.5608937740325901</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.56713998317718</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.57314908504486</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.5788815021514799</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.58429527282714</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.5895235538482599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E5CF-4E20-A17A-7E87AC38DD40}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18942,6 +20231,649 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F911-4323-889F-908444DE1E19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>max_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$A$3:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$K$3:$K$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>9.9500000476837103E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.137079998850822</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22509999573230699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32460001111030501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42588001489639199</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52329999208450295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59850001335143999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66427999734878496</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71943998336791903</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.76304000616073597</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.80261999368667603</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83601999282836903</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86549997329711903</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.88932001590728704</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91127997636795</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.928499996662139</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.938459992408752</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.95231997966766302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95972001552581698</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96634000539779596</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97247999906539895</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.97725999355316095</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.97592002153396595</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.98313999176025302</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.980379998683929</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98677998781204201</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98882001638412398</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98956000804901101</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98721998929977395</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98970001935958796</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.99107998609542802</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.99106001853942804</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99238002300262396</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.99217998981475797</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99414002895355202</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.99459999799728305</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.992919981479644</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99577999114990201</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.99396002292633001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.99503999948501498</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.99481999874114901</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.99672001600265503</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.99448001384735096</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.99518001079559304</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.99615997076034501</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.99533998966216997</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.99548000097274703</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99778002500534002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.99690002202987604</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99779999256134</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.99768000841140703</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.99650001525878895</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.99897998571395796</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.99853998422622603</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.99503999948501498</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.995980024337768</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.998179972171783</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.99699997901916504</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.99742001295089699</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.99676001071929898</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.99746000766754095</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.99819999933242798</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.99713999032974199</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.99760001897811801</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.99786001443862904</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.999040007591247</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.998560011386871</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.99896001815795898</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.99822002649307195</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.99753999710082997</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.99864000082015902</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.99981999397277799</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9673-4C61-94FF-450F3123C822}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21283,6 +23215,649 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5F3E-494B-B03B-26082D18C6CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>max_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$A$3:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>maxgrad_analysis_vgg16_cifar10!$M$3:$M$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.10000000149011599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.207599997520446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28880000114440901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37220001220703097</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48449999094009399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56489998102188099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64649999141693104</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67659997940063399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.718800008296966</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.72409999370574896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.76670002937316895</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76139998435974099</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.765699982643127</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78100001811981201</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.78159999847412098</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.776799976825714</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.78909999132156305</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.79799997806548995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.78399997949600198</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.77270001173019398</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78179997205734197</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.79659998416900601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.787999987602233</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.792400002479553</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.80129998922348</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.79659998416900601</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.79509997367858798</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.79949998855590798</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.79739999771118097</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79350000619888295</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.79659998416900601</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.80250000953674305</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.79430001974105802</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.80879998207092196</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.80110001564025801</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.79769998788833596</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.80150002241134599</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.80430001020431496</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.80809998512268</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.78600001335143999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.80479997396469105</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.80610001087188698</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.792400002479553</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.805899977684021</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.79989999532699496</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.80879998207092196</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.80269998311996404</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.81010001897811801</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.81370002031326205</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.81169998645782404</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.81099998950958196</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.81209999322891202</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.81360000371932895</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.80620002746581998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.80239999294280995</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.80760002136230402</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.81080001592636097</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.80669999122619596</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.79420000314712502</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.80479997396469105</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.80250000953674305</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.80860000848770097</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.80540001392364502</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.80400002002715998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.803699970245361</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.81260001659393299</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.80610001087188698</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.80680000782012895</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.80889999866485596</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.79780000448226895</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.80790001153945901</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.81370002031326205</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.81749999523162797</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.81859999895095803</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.81889998912811202</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.81870001554489102</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.81870001554489102</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.81859999895095803</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.81870001554489102</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.81870001554489102</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.819199979305267</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81950002908706598</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.81959998607635498</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.81940001249313299</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.81940001249313299</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.81950002908706598</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.81989997625350897</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.81999999284744196</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.81989997625350897</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.81999999284744196</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.82010000944137496</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.81999999284744196</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.81999999284744196</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.81980001926422097</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.81980001926422097</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.81989997625350897</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.81999999284744196</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.81989997625350897</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.81980001926422097</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.81970000267028797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7AA1-40D3-9569-358E9F6E90FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -26224,15 +28799,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26262,15 +28837,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:colOff>742949</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26299,16 +28874,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>990599</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>971549</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>109538</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26337,16 +28912,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>933449</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>185738</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>666749</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32092,10 +34667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BF19A8-DA85-42BB-9994-2D295AA2235F}">
-  <dimension ref="A1:M102"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32113,9 +34688,13 @@
     <col min="11" max="11" width="15.7109375" style="20" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" style="20" customWidth="1"/>
     <col min="13" max="13" width="23.5703125" style="21" customWidth="1"/>
+    <col min="14" max="14" width="12" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -32137,8 +34716,14 @@
       <c r="K1" s="33"/>
       <c r="L1" s="33"/>
       <c r="M1" s="34"/>
+      <c r="N1" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="31"/>
     </row>
-    <row r="2" spans="1:13" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37"/>
       <c r="B2" s="13" t="s">
         <v>4</v>
@@ -32176,8 +34761,20 @@
       <c r="M2" s="14" t="s">
         <v>7</v>
       </c>
+      <c r="N2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -32217,8 +34814,20 @@
       <c r="M3" s="17">
         <v>0.10000000149011599</v>
       </c>
+      <c r="N3" s="26">
+        <v>2.3027694225311199</v>
+      </c>
+      <c r="O3" s="26">
+        <v>0.100139997899532</v>
+      </c>
+      <c r="P3" s="26">
+        <v>2.3022925853729199</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>0.10000000149011599</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -32258,8 +34867,20 @@
       <c r="M4" s="17">
         <v>0.207599997520446</v>
       </c>
+      <c r="N4" s="26">
+        <v>2.2586250305175701</v>
+      </c>
+      <c r="O4" s="26">
+        <v>0.149839997291564</v>
+      </c>
+      <c r="P4" s="26">
+        <v>2.0786178112029998</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>0.21170000731944999</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -32299,8 +34920,20 @@
       <c r="M5" s="17">
         <v>0.28880000114440901</v>
       </c>
+      <c r="N5" s="26">
+        <v>1.9639205932617101</v>
+      </c>
+      <c r="O5" s="26">
+        <v>0.25562000274658198</v>
+      </c>
+      <c r="P5" s="26">
+        <v>1.8122906684875399</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0.305900007486343</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -32340,8 +34973,20 @@
       <c r="M6" s="17">
         <v>0.37220001220703097</v>
       </c>
+      <c r="N6" s="26">
+        <v>1.69606614112854</v>
+      </c>
+      <c r="O6" s="26">
+        <v>0.35354000329971302</v>
+      </c>
+      <c r="P6" s="26">
+        <v>1.5514733791351301</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0.41429999470710699</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -32381,8 +35026,20 @@
       <c r="M7" s="17">
         <v>0.48449999094009399</v>
       </c>
+      <c r="N7" s="26">
+        <v>1.4662382602691599</v>
+      </c>
+      <c r="O7" s="26">
+        <v>0.45021998882293701</v>
+      </c>
+      <c r="P7" s="26">
+        <v>1.39426958560943</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0.48269999027252197</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -32422,8 +35079,20 @@
       <c r="M8" s="17">
         <v>0.56489998102188099</v>
       </c>
+      <c r="N8" s="26">
+        <v>1.22249507904052</v>
+      </c>
+      <c r="O8" s="26">
+        <v>0.55084002017974798</v>
+      </c>
+      <c r="P8" s="26">
+        <v>1.1325269937515201</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0.58560001850128096</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -32463,8 +35132,20 @@
       <c r="M9" s="17">
         <v>0.64649999141693104</v>
       </c>
+      <c r="N9" s="26">
+        <v>1.03525698184967</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0.62860000133514404</v>
+      </c>
+      <c r="P9" s="26">
+        <v>1.0254898071289</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0.64120000600814797</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -32504,8 +35185,20 @@
       <c r="M10" s="17">
         <v>0.67659997940063399</v>
       </c>
+      <c r="N10" s="26">
+        <v>0.86408096551895097</v>
+      </c>
+      <c r="O10" s="26">
+        <v>0.691139996051788</v>
+      </c>
+      <c r="P10" s="26">
+        <v>0.89834278821945102</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>0.67890000343322698</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -32545,8 +35238,20 @@
       <c r="M11" s="17">
         <v>0.718800008296966</v>
       </c>
+      <c r="N11" s="26">
+        <v>0.73870247602462702</v>
+      </c>
+      <c r="O11" s="26">
+        <v>0.74011999368667603</v>
+      </c>
+      <c r="P11" s="26">
+        <v>0.83198076486587502</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.71460002660751298</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -32586,8 +35291,20 @@
       <c r="M12" s="17">
         <v>0.72409999370574896</v>
       </c>
+      <c r="N12" s="26">
+        <v>0.62412256002426103</v>
+      </c>
+      <c r="O12" s="26">
+        <v>0.78096002340316695</v>
+      </c>
+      <c r="P12" s="26">
+        <v>0.79875659942626898</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>0.72570002079009999</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -32627,8 +35344,20 @@
       <c r="M13" s="17">
         <v>0.76670002937316895</v>
       </c>
+      <c r="N13" s="26">
+        <v>0.53597235679626398</v>
+      </c>
+      <c r="O13" s="26">
+        <v>0.81419998407363803</v>
+      </c>
+      <c r="P13" s="26">
+        <v>0.72993385791778498</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0.75160002708435003</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>12</v>
       </c>
@@ -32668,8 +35397,20 @@
       <c r="M14" s="17">
         <v>0.76139998435974099</v>
       </c>
+      <c r="N14" s="26">
+        <v>0.43687659502029402</v>
+      </c>
+      <c r="O14" s="26">
+        <v>0.85000002384185702</v>
+      </c>
+      <c r="P14" s="26">
+        <v>0.76859366893768299</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0.754499971866607</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -32709,8 +35450,20 @@
       <c r="M15" s="17">
         <v>0.765699982643127</v>
       </c>
+      <c r="N15" s="26">
+        <v>0.35687324404716397</v>
+      </c>
+      <c r="O15" s="26">
+        <v>0.87647998332977295</v>
+      </c>
+      <c r="P15" s="26">
+        <v>0.722639560699462</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>0.76639997959136896</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>14</v>
       </c>
@@ -32750,8 +35503,20 @@
       <c r="M16" s="17">
         <v>0.78100001811981201</v>
       </c>
+      <c r="N16" s="26">
+        <v>0.296150982379913</v>
+      </c>
+      <c r="O16" s="26">
+        <v>0.89583998918533303</v>
+      </c>
+      <c r="P16" s="26">
+        <v>0.73433947563171298</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>0.76950001716613703</v>
+      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -32791,8 +35556,20 @@
       <c r="M17" s="17">
         <v>0.78159999847412098</v>
       </c>
+      <c r="N17" s="26">
+        <v>0.241215795278549</v>
+      </c>
+      <c r="O17" s="26">
+        <v>0.91596001386642401</v>
+      </c>
+      <c r="P17" s="26">
+        <v>0.86505204439163197</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0.76319998502731301</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -32832,8 +35609,20 @@
       <c r="M18" s="17">
         <v>0.776799976825714</v>
       </c>
+      <c r="N18" s="26">
+        <v>0.20251764357089899</v>
+      </c>
+      <c r="O18" s="26">
+        <v>0.93045997619628895</v>
+      </c>
+      <c r="P18" s="26">
+        <v>0.77807712554931596</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>0.781199991703033</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -32873,8 +35662,20 @@
       <c r="M19" s="17">
         <v>0.78909999132156305</v>
       </c>
+      <c r="N19" s="26">
+        <v>0.159939751029014</v>
+      </c>
+      <c r="O19" s="26">
+        <v>0.94445997476577703</v>
+      </c>
+      <c r="P19" s="26">
+        <v>0.87954413890838601</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>0.776799976825714</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -32914,8 +35715,20 @@
       <c r="M20" s="17">
         <v>0.79799997806548995</v>
       </c>
+      <c r="N20" s="26">
+        <v>0.13020826876163399</v>
+      </c>
+      <c r="O20" s="26">
+        <v>0.95487999916076605</v>
+      </c>
+      <c r="P20" s="26">
+        <v>0.85024952888488703</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>0.77829998731613104</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -32955,8 +35768,20 @@
       <c r="M21" s="17">
         <v>0.78399997949600198</v>
       </c>
+      <c r="N21" s="26">
+        <v>0.113895647227764</v>
+      </c>
+      <c r="O21" s="26">
+        <v>0.96094000339508001</v>
+      </c>
+      <c r="P21" s="26">
+        <v>0.91134178638458196</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>0.78310000896453802</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -32996,8 +35821,20 @@
       <c r="M22" s="17">
         <v>0.77270001173019398</v>
       </c>
+      <c r="N22" s="26">
+        <v>9.8499804735183702E-2</v>
+      </c>
+      <c r="O22" s="26">
+        <v>0.96718001365661599</v>
+      </c>
+      <c r="P22" s="26">
+        <v>0.96869343519210804</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0.77079999446868896</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -33037,8 +35874,20 @@
       <c r="M23" s="17">
         <v>0.78179997205734197</v>
       </c>
+      <c r="N23" s="26">
+        <v>8.3440661430358803E-2</v>
+      </c>
+      <c r="O23" s="26">
+        <v>0.97170001268386796</v>
+      </c>
+      <c r="P23" s="26">
+        <v>0.96055614948272705</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>0.78909999132156305</v>
+      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -33078,8 +35927,20 @@
       <c r="M24" s="17">
         <v>0.79659998416900601</v>
       </c>
+      <c r="N24" s="26">
+        <v>6.3875906169414506E-2</v>
+      </c>
+      <c r="O24" s="26">
+        <v>0.97909998893737704</v>
+      </c>
+      <c r="P24" s="26">
+        <v>0.98949795961380005</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>0.79040002822875899</v>
+      </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -33119,8 +35980,20 @@
       <c r="M25" s="17">
         <v>0.787999987602233</v>
       </c>
+      <c r="N25" s="26">
+        <v>5.7438258081674499E-2</v>
+      </c>
+      <c r="O25" s="26">
+        <v>0.98041999340057295</v>
+      </c>
+      <c r="P25" s="26">
+        <v>1.0180149078369101</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>0.79430001974105802</v>
+      </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -33160,8 +36033,20 @@
       <c r="M26" s="17">
         <v>0.792400002479553</v>
       </c>
+      <c r="N26" s="26">
+        <v>5.1439322531223297E-2</v>
+      </c>
+      <c r="O26" s="26">
+        <v>0.98259997367858798</v>
+      </c>
+      <c r="P26" s="26">
+        <v>0.98585760593414296</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>0.80239999294280995</v>
+      </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>25</v>
       </c>
@@ -33201,8 +36086,20 @@
       <c r="M27" s="17">
         <v>0.80129998922348</v>
       </c>
+      <c r="N27" s="26">
+        <v>4.4517900794744401E-2</v>
+      </c>
+      <c r="O27" s="26">
+        <v>0.98497998714446999</v>
+      </c>
+      <c r="P27" s="26">
+        <v>1.0578082799911499</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>0.79500001668929998</v>
+      </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>26</v>
       </c>
@@ -33242,8 +36139,20 @@
       <c r="M28" s="17">
         <v>0.79659998416900601</v>
       </c>
+      <c r="N28" s="26">
+        <v>4.2967006564140299E-2</v>
+      </c>
+      <c r="O28" s="26">
+        <v>0.98575997352600098</v>
+      </c>
+      <c r="P28" s="26">
+        <v>0.99726057052612305</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>0.79820001125335605</v>
+      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>27</v>
       </c>
@@ -33283,8 +36192,20 @@
       <c r="M29" s="17">
         <v>0.79509997367858798</v>
       </c>
+      <c r="N29" s="26">
+        <v>3.2790429890155702E-2</v>
+      </c>
+      <c r="O29" s="26">
+        <v>0.98913997411727905</v>
+      </c>
+      <c r="P29" s="26">
+        <v>1.1213850975036599</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>0.79369997978210405</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>28</v>
       </c>
@@ -33324,8 +36245,20 @@
       <c r="M30" s="17">
         <v>0.79949998855590798</v>
       </c>
+      <c r="N30" s="26">
+        <v>3.6234069615602403E-2</v>
+      </c>
+      <c r="O30" s="26">
+        <v>0.98783999681472701</v>
+      </c>
+      <c r="P30" s="26">
+        <v>1.1584111452102599</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>0.78250002861022905</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>29</v>
       </c>
@@ -33365,8 +36298,20 @@
       <c r="M31" s="17">
         <v>0.79739999771118097</v>
       </c>
+      <c r="N31" s="26">
+        <v>2.8777642175555201E-2</v>
+      </c>
+      <c r="O31" s="26">
+        <v>0.99011999368667603</v>
+      </c>
+      <c r="P31" s="26">
+        <v>1.1236149072646999</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>0.79309999942779497</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>30</v>
       </c>
@@ -33406,8 +36351,20 @@
       <c r="M32" s="17">
         <v>0.79350000619888295</v>
       </c>
+      <c r="N32" s="26">
+        <v>3.2647304236888802E-2</v>
+      </c>
+      <c r="O32" s="26">
+        <v>0.98916000127792303</v>
+      </c>
+      <c r="P32" s="26">
+        <v>1.08906114101409</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>0.78530001640319802</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>31</v>
       </c>
@@ -33447,8 +36404,20 @@
       <c r="M33" s="17">
         <v>0.79659998416900601</v>
       </c>
+      <c r="N33" s="26">
+        <v>2.5497399270534502E-2</v>
+      </c>
+      <c r="O33" s="26">
+        <v>0.99133998155593805</v>
+      </c>
+      <c r="P33" s="26">
+        <v>1.17526471614837</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>0.79589998722076405</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>32</v>
       </c>
@@ -33488,8 +36457,20 @@
       <c r="M34" s="17">
         <v>0.80250000953674305</v>
       </c>
+      <c r="N34" s="26">
+        <v>2.6842882856726601E-2</v>
+      </c>
+      <c r="O34" s="26">
+        <v>0.99089998006820601</v>
+      </c>
+      <c r="P34" s="26">
+        <v>1.03588771820068</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>0.80180001258850098</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>33</v>
       </c>
@@ -33529,8 +36510,20 @@
       <c r="M35" s="17">
         <v>0.79430001974105802</v>
       </c>
+      <c r="N35" s="26">
+        <v>2.3679494857787999E-2</v>
+      </c>
+      <c r="O35" s="26">
+        <v>0.99181997776031405</v>
+      </c>
+      <c r="P35" s="26">
+        <v>1.16630411148071</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>0.799000024795532</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>34</v>
       </c>
@@ -33570,8 +36563,20 @@
       <c r="M36" s="17">
         <v>0.80879998207092196</v>
       </c>
+      <c r="N36" s="26">
+        <v>1.6706651076674399E-2</v>
+      </c>
+      <c r="O36" s="26">
+        <v>0.99485999345779397</v>
+      </c>
+      <c r="P36" s="26">
+        <v>1.2954134941101001</v>
+      </c>
+      <c r="Q36" s="8">
+        <v>0.77799999713897705</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>35</v>
       </c>
@@ -33611,8 +36616,20 @@
       <c r="M37" s="17">
         <v>0.80110001564025801</v>
       </c>
+      <c r="N37" s="26">
+        <v>2.2398622706532399E-2</v>
+      </c>
+      <c r="O37" s="26">
+        <v>0.99229997396469105</v>
+      </c>
+      <c r="P37" s="26">
+        <v>1.2055369615554801</v>
+      </c>
+      <c r="Q37" s="8">
+        <v>0.79009997844696001</v>
+      </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>36</v>
       </c>
@@ -33652,8 +36669,20 @@
       <c r="M38" s="17">
         <v>0.79769998788833596</v>
       </c>
+      <c r="N38" s="26">
+        <v>1.8463643267750698E-2</v>
+      </c>
+      <c r="O38" s="26">
+        <v>0.99392002820968595</v>
+      </c>
+      <c r="P38" s="26">
+        <v>1.1399447917938199</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>0.79860001802444402</v>
+      </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>37</v>
       </c>
@@ -33693,8 +36722,20 @@
       <c r="M39" s="17">
         <v>0.80150002241134599</v>
       </c>
+      <c r="N39" s="26">
+        <v>1.45105952396988E-2</v>
+      </c>
+      <c r="O39" s="26">
+        <v>0.995119988918304</v>
+      </c>
+      <c r="P39" s="26">
+        <v>1.1890002489089899</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>0.80030000209808305</v>
+      </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>38</v>
       </c>
@@ -33734,8 +36775,20 @@
       <c r="M40" s="17">
         <v>0.80430001020431496</v>
       </c>
+      <c r="N40" s="26">
+        <v>1.9130390137433999E-2</v>
+      </c>
+      <c r="O40" s="26">
+        <v>0.99374002218246404</v>
+      </c>
+      <c r="P40" s="26">
+        <v>1.1808214187621999</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>0.79949998855590798</v>
+      </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>39</v>
       </c>
@@ -33775,8 +36828,20 @@
       <c r="M41" s="17">
         <v>0.80809998512268</v>
       </c>
+      <c r="N41" s="26">
+        <v>1.22592309489846E-2</v>
+      </c>
+      <c r="O41" s="26">
+        <v>0.99599999189376798</v>
+      </c>
+      <c r="P41" s="26">
+        <v>1.2814165353775</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>0.794600009918212</v>
+      </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>40</v>
       </c>
@@ -33816,8 +36881,20 @@
       <c r="M42" s="17">
         <v>0.78600001335143999</v>
       </c>
+      <c r="N42" s="26">
+        <v>1.6287580132484401E-2</v>
+      </c>
+      <c r="O42" s="26">
+        <v>0.994639992713928</v>
+      </c>
+      <c r="P42" s="26">
+        <v>1.1881618499755799</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>0.79809999465942305</v>
+      </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>41</v>
       </c>
@@ -33857,8 +36934,20 @@
       <c r="M43" s="17">
         <v>0.80479997396469105</v>
       </c>
+      <c r="N43" s="26">
+        <v>1.2325801886618099E-2</v>
+      </c>
+      <c r="O43" s="26">
+        <v>0.99615997076034501</v>
+      </c>
+      <c r="P43" s="26">
+        <v>1.2059458494186399</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>0.79790002107620195</v>
+      </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>42</v>
       </c>
@@ -33898,8 +36987,20 @@
       <c r="M44" s="17">
         <v>0.80610001087188698</v>
       </c>
+      <c r="N44" s="26">
+        <v>1.3690935447812001E-2</v>
+      </c>
+      <c r="O44" s="26">
+        <v>0.99554002285003595</v>
+      </c>
+      <c r="P44" s="26">
+        <v>1.25268542766571</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>0.803499996662139</v>
+      </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>43</v>
       </c>
@@ -33939,8 +37040,20 @@
       <c r="M45" s="17">
         <v>0.792400002479553</v>
       </c>
+      <c r="N45" s="26">
+        <v>1.2208929285407E-2</v>
+      </c>
+      <c r="O45" s="26">
+        <v>0.99584001302719105</v>
+      </c>
+      <c r="P45" s="26">
+        <v>1.2093030214309599</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>0.80470001697540205</v>
+      </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>44</v>
       </c>
@@ -33980,8 +37093,20 @@
       <c r="M46" s="17">
         <v>0.805899977684021</v>
       </c>
+      <c r="N46" s="26">
+        <v>1.0713316500186899E-2</v>
+      </c>
+      <c r="O46" s="26">
+        <v>0.99628001451492298</v>
+      </c>
+      <c r="P46" s="26">
+        <v>1.2619669437408401</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>0.80290001630783003</v>
+      </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>45</v>
       </c>
@@ -34021,8 +37146,20 @@
       <c r="M47" s="17">
         <v>0.79989999532699496</v>
       </c>
+      <c r="N47" s="26">
+        <v>1.2847088277339901E-2</v>
+      </c>
+      <c r="O47" s="26">
+        <v>0.99576002359390203</v>
+      </c>
+      <c r="P47" s="26">
+        <v>1.24342000484466</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>0.80010002851486195</v>
+      </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>46</v>
       </c>
@@ -34062,8 +37199,20 @@
       <c r="M48" s="17">
         <v>0.80879998207092196</v>
       </c>
+      <c r="N48" s="26">
+        <v>1.36198019608855E-2</v>
+      </c>
+      <c r="O48" s="26">
+        <v>0.99558001756668002</v>
+      </c>
+      <c r="P48" s="26">
+        <v>1.2116824388503999</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>0.80339998006820601</v>
+      </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>47</v>
       </c>
@@ -34103,8 +37252,20 @@
       <c r="M49" s="17">
         <v>0.80269998311996404</v>
       </c>
+      <c r="N49" s="26">
+        <v>7.8996391966938903E-3</v>
+      </c>
+      <c r="O49" s="26">
+        <v>0.99720001220703103</v>
+      </c>
+      <c r="P49" s="26">
+        <v>1.32473564147949</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>0.80070000886917103</v>
+      </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>48</v>
       </c>
@@ -34144,8 +37305,20 @@
       <c r="M50" s="17">
         <v>0.81010001897811801</v>
       </c>
+      <c r="N50" s="26">
+        <v>1.16662429645657E-2</v>
+      </c>
+      <c r="O50" s="26">
+        <v>0.99594002962112405</v>
+      </c>
+      <c r="P50" s="26">
+        <v>1.3087188005447301</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>0.80339998006820601</v>
+      </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>49</v>
       </c>
@@ -34185,8 +37358,20 @@
       <c r="M51" s="17">
         <v>0.81370002031326205</v>
       </c>
+      <c r="N51" s="26">
+        <v>8.9769149199128099E-3</v>
+      </c>
+      <c r="O51" s="26">
+        <v>0.99672001600265503</v>
+      </c>
+      <c r="P51" s="26">
+        <v>1.29738068580627</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>0.80529999732971103</v>
+      </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>50</v>
       </c>
@@ -34226,8 +37411,20 @@
       <c r="M52" s="17">
         <v>0.81169998645782404</v>
       </c>
+      <c r="N52" s="26">
+        <v>7.7704093419015399E-3</v>
+      </c>
+      <c r="O52" s="26">
+        <v>0.99720001220703103</v>
+      </c>
+      <c r="P52" s="26">
+        <v>1.38581454753875</v>
+      </c>
+      <c r="Q52" s="8">
+        <v>0.79750001430511397</v>
+      </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>51</v>
       </c>
@@ -34267,8 +37464,20 @@
       <c r="M53" s="17">
         <v>0.81099998950958196</v>
       </c>
+      <c r="N53" s="26">
+        <v>1.48136084899306E-2</v>
+      </c>
+      <c r="O53" s="26">
+        <v>0.99519997835159302</v>
+      </c>
+      <c r="P53" s="26">
+        <v>1.18995833396911</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>0.799000024795532</v>
+      </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>52</v>
       </c>
@@ -34308,8 +37517,20 @@
       <c r="M54" s="17">
         <v>0.81209999322891202</v>
       </c>
+      <c r="N54" s="26">
+        <v>7.8989565372467006E-3</v>
+      </c>
+      <c r="O54" s="26">
+        <v>0.99746000766754095</v>
+      </c>
+      <c r="P54" s="26">
+        <v>1.31305539608001</v>
+      </c>
+      <c r="Q54" s="8">
+        <v>0.80159997940063399</v>
+      </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>53</v>
       </c>
@@ -34349,8 +37570,20 @@
       <c r="M55" s="17">
         <v>0.81360000371932895</v>
       </c>
+      <c r="N55" s="26">
+        <v>8.6336946114897693E-3</v>
+      </c>
+      <c r="O55" s="26">
+        <v>0.99698001146316495</v>
+      </c>
+      <c r="P55" s="26">
+        <v>1.27703416347503</v>
+      </c>
+      <c r="Q55" s="8">
+        <v>0.799199998378753</v>
+      </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>54</v>
       </c>
@@ -34390,8 +37623,20 @@
       <c r="M56" s="17">
         <v>0.80620002746581998</v>
       </c>
+      <c r="N56" s="26">
+        <v>1.1168524622917101E-2</v>
+      </c>
+      <c r="O56" s="26">
+        <v>0.99637997150421098</v>
+      </c>
+      <c r="P56" s="26">
+        <v>1.2660480737686099</v>
+      </c>
+      <c r="Q56" s="8">
+        <v>0.80210000276565496</v>
+      </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>55</v>
       </c>
@@ -34431,8 +37676,20 @@
       <c r="M57" s="17">
         <v>0.80239999294280995</v>
       </c>
+      <c r="N57" s="26">
+        <v>9.8036741837859102E-3</v>
+      </c>
+      <c r="O57" s="26">
+        <v>0.99680000543594305</v>
+      </c>
+      <c r="P57" s="26">
+        <v>1.3768168687820399</v>
+      </c>
+      <c r="Q57" s="8">
+        <v>0.79860001802444402</v>
+      </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>56</v>
       </c>
@@ -34472,8 +37729,20 @@
       <c r="M58" s="17">
         <v>0.80760002136230402</v>
       </c>
+      <c r="N58" s="26">
+        <v>8.66168364882469E-3</v>
+      </c>
+      <c r="O58" s="26">
+        <v>0.99742001295089699</v>
+      </c>
+      <c r="P58" s="26">
+        <v>1.2122414112091</v>
+      </c>
+      <c r="Q58" s="8">
+        <v>0.799000024795532</v>
+      </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>57</v>
       </c>
@@ -34513,8 +37782,20 @@
       <c r="M59" s="17">
         <v>0.81080001592636097</v>
       </c>
+      <c r="N59" s="26">
+        <v>6.0448790900409204E-3</v>
+      </c>
+      <c r="O59" s="26">
+        <v>0.99805998802185003</v>
+      </c>
+      <c r="P59" s="26">
+        <v>1.3161154985427801</v>
+      </c>
+      <c r="Q59" s="8">
+        <v>0.78600001335143999</v>
+      </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>58</v>
       </c>
@@ -34554,8 +37835,20 @@
       <c r="M60" s="17">
         <v>0.80669999122619596</v>
       </c>
+      <c r="N60" s="26">
+        <v>9.3184653669595701E-3</v>
+      </c>
+      <c r="O60" s="26">
+        <v>0.99708002805709794</v>
+      </c>
+      <c r="P60" s="26">
+        <v>1.2984709739685001</v>
+      </c>
+      <c r="Q60" s="8">
+        <v>0.79799997806548995</v>
+      </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>59</v>
       </c>
@@ -34595,8 +37888,20 @@
       <c r="M61" s="17">
         <v>0.79420000314712502</v>
       </c>
+      <c r="N61" s="26">
+        <v>6.3734287396073298E-3</v>
+      </c>
+      <c r="O61" s="26">
+        <v>0.99786001443862904</v>
+      </c>
+      <c r="P61" s="26">
+        <v>1.32701575756073</v>
+      </c>
+      <c r="Q61" s="8">
+        <v>0.79659998416900601</v>
+      </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>60</v>
       </c>
@@ -34636,8 +37941,20 @@
       <c r="M62" s="17">
         <v>0.80479997396469105</v>
       </c>
+      <c r="N62" s="26">
+        <v>1.1314079165458599E-2</v>
+      </c>
+      <c r="O62" s="26">
+        <v>0.99615997076034501</v>
+      </c>
+      <c r="P62" s="26">
+        <v>1.23300921916961</v>
+      </c>
+      <c r="Q62" s="8">
+        <v>0.80210000276565496</v>
+      </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>61</v>
       </c>
@@ -34677,8 +37994,20 @@
       <c r="M63" s="17">
         <v>0.80250000953674305</v>
       </c>
+      <c r="N63" s="26">
+        <v>4.1706529445946199E-3</v>
+      </c>
+      <c r="O63" s="26">
+        <v>0.99864000082015902</v>
+      </c>
+      <c r="P63" s="26">
+        <v>1.40980112552642</v>
+      </c>
+      <c r="Q63" s="8">
+        <v>0.80299997329711903</v>
+      </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>62</v>
       </c>
@@ -34718,8 +38047,20 @@
       <c r="M64" s="17">
         <v>0.80860000848770097</v>
       </c>
+      <c r="N64" s="26">
+        <v>7.7819828875362804E-3</v>
+      </c>
+      <c r="O64" s="26">
+        <v>0.99753999710082997</v>
+      </c>
+      <c r="P64" s="26">
+        <v>1.3081873655319201</v>
+      </c>
+      <c r="Q64" s="8">
+        <v>0.80150002241134599</v>
+      </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>63</v>
       </c>
@@ -34759,8 +38100,20 @@
       <c r="M65" s="17">
         <v>0.80540001392364502</v>
       </c>
+      <c r="N65" s="26">
+        <v>1.6465428052469999E-3</v>
+      </c>
+      <c r="O65" s="26">
+        <v>0.99949997663497903</v>
+      </c>
+      <c r="P65" s="26">
+        <v>1.4868196249008101</v>
+      </c>
+      <c r="Q65" s="8">
+        <v>0.80620002746581998</v>
+      </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>64</v>
       </c>
@@ -34800,8 +38153,20 @@
       <c r="M66" s="17">
         <v>0.80400002002715998</v>
       </c>
+      <c r="N66" s="26">
+        <v>4.7559421509504301E-3</v>
+      </c>
+      <c r="O66" s="26">
+        <v>0.99852001667022705</v>
+      </c>
+      <c r="P66" s="26">
+        <v>1.3691926002502399</v>
+      </c>
+      <c r="Q66" s="8">
+        <v>0.80970001220703103</v>
+      </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>65</v>
       </c>
@@ -34841,8 +38206,20 @@
       <c r="M67" s="17">
         <v>0.803699970245361</v>
       </c>
+      <c r="N67" s="26">
+        <v>3.5061445087194399E-3</v>
+      </c>
+      <c r="O67" s="26">
+        <v>0.998759984970092</v>
+      </c>
+      <c r="P67" s="26">
+        <v>1.64860951900482</v>
+      </c>
+      <c r="Q67" s="8">
+        <v>0.79280000925063998</v>
+      </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>66</v>
       </c>
@@ -34882,8 +38259,20 @@
       <c r="M68" s="17">
         <v>0.81260001659393299</v>
       </c>
+      <c r="N68" s="26">
+        <v>1.09932459890842E-2</v>
+      </c>
+      <c r="O68" s="26">
+        <v>0.996360003948211</v>
+      </c>
+      <c r="P68" s="26">
+        <v>1.2998180389404199</v>
+      </c>
+      <c r="Q68" s="8">
+        <v>0.80169999599456698</v>
+      </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>67</v>
       </c>
@@ -34923,8 +38312,20 @@
       <c r="M69" s="17">
         <v>0.80610001087188698</v>
       </c>
+      <c r="N69" s="26">
+        <v>4.3701562099158703E-3</v>
+      </c>
+      <c r="O69" s="26">
+        <v>0.99860000610351496</v>
+      </c>
+      <c r="P69" s="26">
+        <v>1.52765369415283</v>
+      </c>
+      <c r="Q69" s="8">
+        <v>0.79809999465942305</v>
+      </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>68</v>
       </c>
@@ -34964,8 +38365,20 @@
       <c r="M70" s="17">
         <v>0.80680000782012895</v>
       </c>
+      <c r="N70" s="26">
+        <v>8.7748803198337503E-3</v>
+      </c>
+      <c r="O70" s="26">
+        <v>0.99695998430251997</v>
+      </c>
+      <c r="P70" s="26">
+        <v>1.2738339900970399</v>
+      </c>
+      <c r="Q70" s="8">
+        <v>0.80460000038146895</v>
+      </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>69</v>
       </c>
@@ -35005,8 +38418,20 @@
       <c r="M71" s="17">
         <v>0.80889999866485596</v>
       </c>
+      <c r="N71" s="26">
+        <v>5.3161205723881704E-3</v>
+      </c>
+      <c r="O71" s="26">
+        <v>0.99823999404907204</v>
+      </c>
+      <c r="P71" s="26">
+        <v>1.36833119392395</v>
+      </c>
+      <c r="Q71" s="8">
+        <v>0.79710000753402699</v>
+      </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
         <v>70</v>
       </c>
@@ -35046,8 +38471,20 @@
       <c r="M72" s="17">
         <v>0.79780000448226895</v>
       </c>
+      <c r="N72" s="26">
+        <v>5.2651176229119301E-3</v>
+      </c>
+      <c r="O72" s="26">
+        <v>0.99834001064300504</v>
+      </c>
+      <c r="P72" s="26">
+        <v>1.3437414169311499</v>
+      </c>
+      <c r="Q72" s="8">
+        <v>0.80470001697540205</v>
+      </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="12">
         <v>71</v>
       </c>
@@ -35087,8 +38524,20 @@
       <c r="M73" s="17">
         <v>0.80790001153945901</v>
       </c>
+      <c r="N73" s="26">
+        <v>3.2543926499783902E-3</v>
+      </c>
+      <c r="O73" s="26">
+        <v>0.99893999099731401</v>
+      </c>
+      <c r="P73" s="26">
+        <v>1.41374015808105</v>
+      </c>
+      <c r="Q73" s="8">
+        <v>0.79790002107620195</v>
+      </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>72</v>
       </c>
@@ -35128,8 +38577,20 @@
       <c r="M74" s="17">
         <v>0.81370002031326205</v>
       </c>
+      <c r="N74" s="26">
+        <v>4.1170655749738199E-3</v>
+      </c>
+      <c r="O74" s="26">
+        <v>0.99871999025344804</v>
+      </c>
+      <c r="P74" s="26">
+        <v>1.4031784534454299</v>
+      </c>
+      <c r="Q74" s="8">
+        <v>0.80879998207092196</v>
+      </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>73</v>
       </c>
@@ -35169,8 +38630,20 @@
       <c r="M75" s="17">
         <v>0.81749999523162797</v>
       </c>
+      <c r="N75" s="26">
+        <v>7.5495112687349302E-3</v>
+      </c>
+      <c r="O75" s="26">
+        <v>0.99756002426147405</v>
+      </c>
+      <c r="P75" s="26">
+        <v>1.35831654071807</v>
+      </c>
+      <c r="Q75" s="8">
+        <v>0.80049997568130404</v>
+      </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>74</v>
       </c>
@@ -35210,8 +38683,20 @@
       <c r="M76" s="17">
         <v>0.81859999895095803</v>
       </c>
+      <c r="N76" s="26">
+        <v>8.2901436835527403E-3</v>
+      </c>
+      <c r="O76" s="26">
+        <v>0.99720001220703103</v>
+      </c>
+      <c r="P76" s="26">
+        <v>1.3287324905395499</v>
+      </c>
+      <c r="Q76" s="8">
+        <v>0.80669999122619596</v>
+      </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>75</v>
       </c>
@@ -35251,8 +38736,20 @@
       <c r="M77" s="17">
         <v>0.81889998912811202</v>
       </c>
+      <c r="N77" s="26">
+        <v>3.2806065864860998E-3</v>
+      </c>
+      <c r="O77" s="26">
+        <v>0.99908000230789096</v>
+      </c>
+      <c r="P77" s="26">
+        <v>1.46714067459106</v>
+      </c>
+      <c r="Q77" s="8">
+        <v>0.79500001668929998</v>
+      </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>76</v>
       </c>
@@ -35292,8 +38789,20 @@
       <c r="M78" s="17">
         <v>0.81870001554489102</v>
       </c>
+      <c r="N78" s="26">
+        <v>4.3930583633482404E-3</v>
+      </c>
+      <c r="O78" s="26">
+        <v>0.99848002195358199</v>
+      </c>
+      <c r="P78" s="26">
+        <v>1.4421035051345801</v>
+      </c>
+      <c r="Q78" s="8">
+        <v>0.79699999094009399</v>
+      </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>77</v>
       </c>
@@ -35333,8 +38842,20 @@
       <c r="M79" s="17">
         <v>0.81870001554489102</v>
       </c>
+      <c r="N79" s="26">
+        <v>7.9995980486273696E-3</v>
+      </c>
+      <c r="O79" s="26">
+        <v>0.99761998653411799</v>
+      </c>
+      <c r="P79" s="26">
+        <v>1.3833097219467101</v>
+      </c>
+      <c r="Q79" s="8">
+        <v>0.80199998617172197</v>
+      </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>78</v>
       </c>
@@ -35374,8 +38895,20 @@
       <c r="M80" s="17">
         <v>0.81859999895095803</v>
       </c>
+      <c r="N80" s="26">
+        <v>2.0557285752147401E-3</v>
+      </c>
+      <c r="O80" s="26">
+        <v>0.99927997589111295</v>
+      </c>
+      <c r="P80" s="26">
+        <v>1.4210299253463701</v>
+      </c>
+      <c r="Q80" s="8">
+        <v>0.80449998378753595</v>
+      </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
         <v>79</v>
       </c>
@@ -35415,8 +38948,20 @@
       <c r="M81" s="17">
         <v>0.81870001554489102</v>
       </c>
+      <c r="N81" s="26">
+        <v>2.5057077873498201E-3</v>
+      </c>
+      <c r="O81" s="26">
+        <v>0.99919998645782404</v>
+      </c>
+      <c r="P81" s="26">
+        <v>1.44810795783996</v>
+      </c>
+      <c r="Q81" s="8">
+        <v>0.80430001020431496</v>
+      </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>80</v>
       </c>
@@ -35456,8 +39001,20 @@
       <c r="M82" s="17">
         <v>0.81870001554489102</v>
       </c>
+      <c r="N82" s="26">
+        <v>4.9772616475820498E-3</v>
+      </c>
+      <c r="O82" s="26">
+        <v>0.99830001592636097</v>
+      </c>
+      <c r="P82" s="26">
+        <v>1.4834080934524501</v>
+      </c>
+      <c r="Q82" s="8">
+        <v>0.80320000648498502</v>
+      </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
         <v>81</v>
       </c>
@@ -35497,8 +39054,20 @@
       <c r="M83" s="17">
         <v>0.819199979305267</v>
       </c>
+      <c r="N83" s="26">
+        <v>7.8713977709412505E-3</v>
+      </c>
+      <c r="O83" s="26">
+        <v>0.99786001443862904</v>
+      </c>
+      <c r="P83" s="26">
+        <v>1.26602470874786</v>
+      </c>
+      <c r="Q83" s="8">
+        <v>0.80970001220703103</v>
+      </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>82</v>
       </c>
@@ -35538,8 +39107,20 @@
       <c r="M84" s="17">
         <v>0.81950002908706598</v>
       </c>
+      <c r="N84" s="26">
+        <v>9.0218998957425302E-4</v>
+      </c>
+      <c r="O84" s="26">
+        <v>0.99974000453948897</v>
+      </c>
+      <c r="P84" s="26">
+        <v>1.39194107055664</v>
+      </c>
+      <c r="Q84" s="8">
+        <v>0.80970001220703103</v>
+      </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
         <v>83</v>
       </c>
@@ -35579,8 +39160,20 @@
       <c r="M85" s="17">
         <v>0.81959998607635498</v>
       </c>
+      <c r="N85" s="26">
+        <v>1.39324998599477E-4</v>
+      </c>
+      <c r="O85" s="26">
+        <v>1</v>
+      </c>
+      <c r="P85" s="26">
+        <v>1.4401205778121899</v>
+      </c>
+      <c r="Q85" s="8">
+        <v>0.81220000982284501</v>
+      </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
         <v>84</v>
       </c>
@@ -35620,8 +39213,20 @@
       <c r="M86" s="17">
         <v>0.81940001249313299</v>
       </c>
+      <c r="N86" s="27">
+        <v>2.3290514945983799E-5</v>
+      </c>
+      <c r="O86" s="26">
+        <v>1</v>
+      </c>
+      <c r="P86" s="26">
+        <v>1.4550211429595901</v>
+      </c>
+      <c r="Q86" s="8">
+        <v>0.81379997730255105</v>
+      </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
         <v>85</v>
       </c>
@@ -35661,8 +39266,20 @@
       <c r="M87" s="17">
         <v>0.81940001249313299</v>
       </c>
+      <c r="N87" s="27">
+        <v>1.4991532225394599E-5</v>
+      </c>
+      <c r="O87" s="26">
+        <v>1</v>
+      </c>
+      <c r="P87" s="26">
+        <v>1.46996474266052</v>
+      </c>
+      <c r="Q87" s="8">
+        <v>0.81440001726150502</v>
+      </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="12">
         <v>86</v>
       </c>
@@ -35702,8 +39319,20 @@
       <c r="M88" s="17">
         <v>0.81950002908706598</v>
       </c>
+      <c r="N88" s="27">
+        <v>1.22376850413274E-5</v>
+      </c>
+      <c r="O88" s="26">
+        <v>1</v>
+      </c>
+      <c r="P88" s="26">
+        <v>1.4829174280166599</v>
+      </c>
+      <c r="Q88" s="8">
+        <v>0.81410002708435003</v>
+      </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="12">
         <v>87</v>
       </c>
@@ -35743,8 +39372,20 @@
       <c r="M89" s="17">
         <v>0.81989997625350897</v>
       </c>
+      <c r="N89" s="27">
+        <v>1.04406317404937E-5</v>
+      </c>
+      <c r="O89" s="26">
+        <v>1</v>
+      </c>
+      <c r="P89" s="26">
+        <v>1.49461674690246</v>
+      </c>
+      <c r="Q89" s="8">
+        <v>0.81419998407363803</v>
+      </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
         <v>88</v>
       </c>
@@ -35784,8 +39425,20 @@
       <c r="M90" s="17">
         <v>0.81999999284744196</v>
       </c>
+      <c r="N90" s="27">
+        <v>9.1319379862397892E-6</v>
+      </c>
+      <c r="O90" s="26">
+        <v>1</v>
+      </c>
+      <c r="P90" s="26">
+        <v>1.5052117109298699</v>
+      </c>
+      <c r="Q90" s="8">
+        <v>0.81449997425079301</v>
+      </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
         <v>89</v>
       </c>
@@ -35825,8 +39478,20 @@
       <c r="M91" s="17">
         <v>0.81989997625350897</v>
       </c>
+      <c r="N91" s="27">
+        <v>8.1310226960340498E-6</v>
+      </c>
+      <c r="O91" s="26">
+        <v>1</v>
+      </c>
+      <c r="P91" s="26">
+        <v>1.5148837566375699</v>
+      </c>
+      <c r="Q91" s="8">
+        <v>0.81440001726150502</v>
+      </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>90</v>
       </c>
@@ -35866,8 +39531,20 @@
       <c r="M92" s="17">
         <v>0.81999999284744196</v>
       </c>
+      <c r="N92" s="27">
+        <v>7.3339556365681304E-6</v>
+      </c>
+      <c r="O92" s="26">
+        <v>1</v>
+      </c>
+      <c r="P92" s="26">
+        <v>1.52382004261016</v>
+      </c>
+      <c r="Q92" s="8">
+        <v>0.81459999084472601</v>
+      </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>91</v>
       </c>
@@ -35907,8 +39584,20 @@
       <c r="M93" s="17">
         <v>0.82010000944137496</v>
       </c>
+      <c r="N93" s="27">
+        <v>6.6808324845624097E-6</v>
+      </c>
+      <c r="O93" s="26">
+        <v>1</v>
+      </c>
+      <c r="P93" s="26">
+        <v>1.5321733951568599</v>
+      </c>
+      <c r="Q93" s="8">
+        <v>0.81449997425079301</v>
+      </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="12">
         <v>92</v>
       </c>
@@ -35948,8 +39637,20 @@
       <c r="M94" s="17">
         <v>0.81999999284744196</v>
       </c>
+      <c r="N94" s="27">
+        <v>6.1339046624197997E-6</v>
+      </c>
+      <c r="O94" s="26">
+        <v>1</v>
+      </c>
+      <c r="P94" s="26">
+        <v>1.5400135517120299</v>
+      </c>
+      <c r="Q94" s="8">
+        <v>0.81459999084472601</v>
+      </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="12">
         <v>93</v>
       </c>
@@ -35989,8 +39690,20 @@
       <c r="M95" s="17">
         <v>0.81999999284744196</v>
       </c>
+      <c r="N95" s="27">
+        <v>5.6691937970754199E-6</v>
+      </c>
+      <c r="O95" s="26">
+        <v>1</v>
+      </c>
+      <c r="P95" s="26">
+        <v>1.5473601818084699</v>
+      </c>
+      <c r="Q95" s="8">
+        <v>0.81459999084472601</v>
+      </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="12">
         <v>94</v>
       </c>
@@ -36030,8 +39743,20 @@
       <c r="M96" s="17">
         <v>0.81980001926422097</v>
       </c>
+      <c r="N96" s="27">
+        <v>5.2707268878293596E-6</v>
+      </c>
+      <c r="O96" s="26">
+        <v>1</v>
+      </c>
+      <c r="P96" s="26">
+        <v>1.5543675422668399</v>
+      </c>
+      <c r="Q96" s="8">
+        <v>0.814800024032592</v>
+      </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="12">
         <v>95</v>
       </c>
@@ -36071,8 +39796,20 @@
       <c r="M97" s="17">
         <v>0.81980001926422097</v>
       </c>
+      <c r="N97" s="27">
+        <v>4.9238369683734996E-6</v>
+      </c>
+      <c r="O97" s="26">
+        <v>1</v>
+      </c>
+      <c r="P97" s="26">
+        <v>1.5608937740325901</v>
+      </c>
+      <c r="Q97" s="8">
+        <v>0.81510001420974698</v>
+      </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="12">
         <v>96</v>
       </c>
@@ -36112,8 +39849,20 @@
       <c r="M98" s="17">
         <v>0.81989997625350897</v>
       </c>
+      <c r="N98" s="27">
+        <v>4.6196814764698502E-6</v>
+      </c>
+      <c r="O98" s="26">
+        <v>1</v>
+      </c>
+      <c r="P98" s="26">
+        <v>1.56713998317718</v>
+      </c>
+      <c r="Q98" s="8">
+        <v>0.81510001420974698</v>
+      </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="12">
         <v>97</v>
       </c>
@@ -36153,8 +39902,20 @@
       <c r="M99" s="17">
         <v>0.81999999284744196</v>
       </c>
+      <c r="N99" s="27">
+        <v>4.3496561374922698E-6</v>
+      </c>
+      <c r="O99" s="26">
+        <v>1</v>
+      </c>
+      <c r="P99" s="26">
+        <v>1.57314908504486</v>
+      </c>
+      <c r="Q99" s="8">
+        <v>0.81499999761581399</v>
+      </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="12">
         <v>98</v>
       </c>
@@ -36194,8 +39955,20 @@
       <c r="M100" s="17">
         <v>0.81989997625350897</v>
       </c>
+      <c r="N100" s="27">
+        <v>4.1098924157267902E-6</v>
+      </c>
+      <c r="O100" s="26">
+        <v>1</v>
+      </c>
+      <c r="P100" s="26">
+        <v>1.5788815021514799</v>
+      </c>
+      <c r="Q100" s="8">
+        <v>0.81489998102188099</v>
+      </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="12">
         <v>99</v>
       </c>
@@ -36235,8 +40008,20 @@
       <c r="M101" s="17">
         <v>0.81980001926422097</v>
       </c>
+      <c r="N101" s="27">
+        <v>3.8948614928813101E-6</v>
+      </c>
+      <c r="O101" s="26">
+        <v>1</v>
+      </c>
+      <c r="P101" s="26">
+        <v>1.58429527282714</v>
+      </c>
+      <c r="Q101" s="8">
+        <v>0.814800024032592</v>
+      </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>100</v>
       </c>
@@ -36276,13 +40061,26 @@
       <c r="M102" s="17">
         <v>0.81970000267028797</v>
       </c>
+      <c r="N102" s="27">
+        <v>3.7005947888246699E-6</v>
+      </c>
+      <c r="O102" s="26">
+        <v>1</v>
+      </c>
+      <c r="P102" s="26">
+        <v>1.5895235538482599</v>
+      </c>
+      <c r="Q102" s="8">
+        <v>0.814800024032592</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>